<commit_message>
Add labels and custom colours to plots
</commit_message>
<xml_diff>
--- a/data/Crossing data summary A_2072 B_1590 - CLEAN.xlsx
+++ b/data/Crossing data summary A_2072 B_1590 - CLEAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ueahome\eressci1\hpd08ucu\data\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ECD0AF-4030-47C7-BDB7-B05753671C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C750A9C3-E08F-4A71-AA45-584E41CF22E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F1" sheetId="1" r:id="rId1"/>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="44">
   <si>
     <t>Genotype count/percentage</t>
   </si>
@@ -8681,18 +8681,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="E42:N42"/>
+    <mergeCell ref="Q42:T42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="E100:N100"/>
     <mergeCell ref="Q100:T100"/>
     <mergeCell ref="V100:Y100"/>
     <mergeCell ref="E119:N119"/>
     <mergeCell ref="Q119:T119"/>
     <mergeCell ref="V119:Y119"/>
-    <mergeCell ref="E3:N3"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="E42:N42"/>
-    <mergeCell ref="Q42:T42"/>
-    <mergeCell ref="V42:Y42"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8703,10 +8703,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86A2A7A-BD28-4849-8891-7A79FC23407A}">
-  <dimension ref="C3:Y147"/>
+  <dimension ref="C3:AA147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147:AA147"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD10" sqref="AD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8720,7 +8720,7 @@
     <col min="23" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -8752,8 +8752,11 @@
         <v>24</v>
       </c>
       <c r="Y3" s="1"/>
-    </row>
-    <row r="4" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
@@ -8818,7 +8821,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
@@ -8892,8 +8895,11 @@
         <f>(V5/N5)*100</f>
         <v>22.222222222222221</v>
       </c>
-    </row>
-    <row r="6" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA5" s="4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D6" s="4">
         <v>2</v>
       </c>
@@ -8917,7 +8923,7 @@
         <v>103</v>
       </c>
       <c r="K6" s="10">
-        <f t="shared" ref="K6:K50" si="1">J6/O6*100</f>
+        <f t="shared" ref="K6:K45" si="1">J6/O6*100</f>
         <v>96.261682242990659</v>
       </c>
       <c r="L6" s="4">
@@ -8925,7 +8931,7 @@
         <v>59</v>
       </c>
       <c r="M6" s="10">
-        <f t="shared" ref="M6:M50" si="3">L6/O6*100</f>
+        <f t="shared" ref="M6:M45" si="3">L6/O6*100</f>
         <v>55.140186915887845</v>
       </c>
       <c r="N6" s="4">
@@ -8964,8 +8970,11 @@
         <f t="shared" ref="Y6:Y45" si="9">(V6/N6)*100</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA6" s="4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D7" s="4">
         <v>3</v>
       </c>
@@ -8977,7 +8986,7 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
     </row>
-    <row r="8" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D8" s="4">
         <v>4</v>
       </c>
@@ -8989,7 +8998,7 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
     </row>
-    <row r="9" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D9" s="4">
         <v>5</v>
       </c>
@@ -9047,8 +9056,11 @@
         <v>100</v>
       </c>
       <c r="Y9" s="10"/>
-    </row>
-    <row r="10" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA9" s="4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D10" s="4">
         <v>6</v>
       </c>
@@ -9060,7 +9072,7 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
     </row>
-    <row r="11" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D11" s="4">
         <v>7</v>
       </c>
@@ -9118,8 +9130,11 @@
         <v>100</v>
       </c>
       <c r="Y11" s="10"/>
-    </row>
-    <row r="12" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA11" s="4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D12" s="4">
         <v>8</v>
       </c>
@@ -9186,8 +9201,11 @@
         <f t="shared" si="9"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA12" s="4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D13" s="4">
         <v>9</v>
       </c>
@@ -9258,8 +9276,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA13" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D14" s="4">
         <v>10</v>
       </c>
@@ -9271,7 +9292,7 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
     </row>
-    <row r="15" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D15" s="4">
         <v>11</v>
       </c>
@@ -9283,7 +9304,7 @@
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
     </row>
-    <row r="16" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D16" s="4">
         <v>12</v>
       </c>
@@ -9295,7 +9316,7 @@
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
     </row>
-    <row r="17" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D17" s="4">
         <v>13</v>
       </c>
@@ -9362,8 +9383,11 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA17" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D18" s="4">
         <v>14</v>
       </c>
@@ -9434,8 +9458,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA18" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D19" s="4">
         <v>15</v>
       </c>
@@ -9502,8 +9529,11 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA19" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D20" s="4">
         <v>16</v>
       </c>
@@ -9515,7 +9545,7 @@
       <c r="X20" s="10"/>
       <c r="Y20" s="10"/>
     </row>
-    <row r="21" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D21" s="4">
         <v>17</v>
       </c>
@@ -9573,8 +9603,11 @@
         <v>100</v>
       </c>
       <c r="Y21" s="10"/>
-    </row>
-    <row r="22" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA21" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D22" s="4">
         <v>18</v>
       </c>
@@ -9586,7 +9619,7 @@
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
     </row>
-    <row r="23" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D23" s="4">
         <v>19</v>
       </c>
@@ -9598,7 +9631,7 @@
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
     </row>
-    <row r="24" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D24" s="4">
         <v>20</v>
       </c>
@@ -9610,7 +9643,7 @@
       <c r="X24" s="10"/>
       <c r="Y24" s="10"/>
     </row>
-    <row r="25" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D25" s="4">
         <v>21</v>
       </c>
@@ -9681,8 +9714,11 @@
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA25" s="4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D26" s="4">
         <v>22</v>
       </c>
@@ -9694,7 +9730,7 @@
       <c r="X26" s="10"/>
       <c r="Y26" s="10"/>
     </row>
-    <row r="27" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D27" s="4">
         <v>23</v>
       </c>
@@ -9706,7 +9742,7 @@
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
     </row>
-    <row r="28" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D28" s="4">
         <v>24</v>
       </c>
@@ -9777,8 +9813,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA28" s="4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D29" s="4">
         <v>25</v>
       </c>
@@ -9845,8 +9884,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA29" s="4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D30" s="4">
         <v>26</v>
       </c>
@@ -9913,8 +9955,11 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA30" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D31" s="4">
         <v>27</v>
       </c>
@@ -9985,8 +10030,11 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA31" s="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D32" s="4">
         <v>28</v>
       </c>
@@ -10057,8 +10105,11 @@
         <f t="shared" si="9"/>
         <v>14.285714285714285</v>
       </c>
-    </row>
-    <row r="33" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA32" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D33" s="4">
         <v>29</v>
       </c>
@@ -10070,7 +10121,7 @@
       <c r="X33" s="10"/>
       <c r="Y33" s="10"/>
     </row>
-    <row r="34" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D34" s="4">
         <v>30</v>
       </c>
@@ -10082,7 +10133,7 @@
       <c r="X34" s="10"/>
       <c r="Y34" s="10"/>
     </row>
-    <row r="35" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D35" s="4">
         <v>31</v>
       </c>
@@ -10140,8 +10191,11 @@
         <v>100</v>
       </c>
       <c r="Y35" s="10"/>
-    </row>
-    <row r="36" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA35" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <v>32</v>
       </c>
@@ -10153,7 +10207,7 @@
       <c r="X36" s="10"/>
       <c r="Y36" s="10"/>
     </row>
-    <row r="37" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D37" s="4">
         <v>33</v>
       </c>
@@ -10211,8 +10265,11 @@
         <v>100</v>
       </c>
       <c r="Y37" s="10"/>
-    </row>
-    <row r="38" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA37" s="4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D38" s="4">
         <v>34</v>
       </c>
@@ -10224,7 +10281,7 @@
       <c r="X38" s="10"/>
       <c r="Y38" s="10"/>
     </row>
-    <row r="39" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D39" s="4">
         <v>35</v>
       </c>
@@ -10291,8 +10348,11 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA39" s="4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D40" s="4">
         <v>36</v>
       </c>
@@ -10304,7 +10364,7 @@
       <c r="X40" s="10"/>
       <c r="Y40" s="10"/>
     </row>
-    <row r="41" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D41" s="4">
         <v>37</v>
       </c>
@@ -10371,8 +10431,11 @@
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="42" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA41" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D42" s="4">
         <v>38</v>
       </c>
@@ -10384,7 +10447,7 @@
       <c r="X42" s="10"/>
       <c r="Y42" s="10"/>
     </row>
-    <row r="43" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D43" s="4">
         <v>39</v>
       </c>
@@ -10396,7 +10459,7 @@
       <c r="X43" s="10"/>
       <c r="Y43" s="10"/>
     </row>
-    <row r="44" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D44" s="4">
         <v>40</v>
       </c>
@@ -10467,8 +10530,11 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="45" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA44" s="4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D45" s="4">
         <v>41</v>
       </c>
@@ -10535,8 +10601,11 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="46" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA45" s="4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D46" s="4">
         <v>42</v>
       </c>
@@ -10544,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D47" s="4">
         <v>43</v>
       </c>
@@ -10552,7 +10621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D48" s="4">
         <v>44</v>
       </c>
@@ -10560,7 +10629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D49" s="4">
         <v>45</v>
       </c>
@@ -10568,13 +10637,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:27" x14ac:dyDescent="0.25">
       <c r="K50" s="6"/>
       <c r="M50" s="6"/>
       <c r="X50" s="6"/>
       <c r="Y50" s="6"/>
     </row>
-    <row r="52" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="14"/>
@@ -10598,7 +10667,7 @@
       <c r="X52" s="1"/>
       <c r="Y52" s="1"/>
     </row>
-    <row r="53" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -10622,7 +10691,7 @@
       <c r="X53" s="1"/>
       <c r="Y53" s="1"/>
     </row>
-    <row r="54" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C54" s="4" t="s">
         <v>28</v>
       </c>
@@ -10683,8 +10752,11 @@
         <v>100</v>
       </c>
       <c r="Y54" s="10"/>
-    </row>
-    <row r="55" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA54" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D55" s="4">
         <v>2</v>
       </c>
@@ -10696,7 +10768,7 @@
       <c r="X55" s="10"/>
       <c r="Y55" s="10"/>
     </row>
-    <row r="56" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D56" s="4">
         <v>3</v>
       </c>
@@ -10720,7 +10792,7 @@
         <v>45</v>
       </c>
       <c r="K56" s="10">
-        <f t="shared" ref="K56:K99" si="11">(J56/O56)*100</f>
+        <f t="shared" ref="K56:K98" si="11">(J56/O56)*100</f>
         <v>71.428571428571431</v>
       </c>
       <c r="L56" s="4">
@@ -10728,7 +10800,7 @@
         <v>35</v>
       </c>
       <c r="M56" s="10">
-        <f t="shared" ref="M56:M99" si="13">(L56/O56)*100</f>
+        <f t="shared" ref="M56:M98" si="13">(L56/O56)*100</f>
         <v>55.555555555555557</v>
       </c>
       <c r="N56" s="4">
@@ -10756,19 +10828,22 @@
         <v>18</v>
       </c>
       <c r="W56" s="4">
-        <f t="shared" ref="W56:W99" si="17">SUM(R56:U56)</f>
+        <f t="shared" ref="W56:W98" si="17">SUM(R56:U56)</f>
         <v>63</v>
       </c>
       <c r="X56" s="10">
-        <f t="shared" ref="X56:X99" si="18">(W56/O56)*100</f>
+        <f t="shared" ref="X56:X98" si="18">(W56/O56)*100</f>
         <v>100</v>
       </c>
       <c r="Y56" s="10">
-        <f t="shared" ref="Y56:Y99" si="19">(V56/N56)*100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="3:25" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Y56:Y94" si="19">(V56/N56)*100</f>
+        <v>100</v>
+      </c>
+      <c r="AA56" s="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D57" s="4">
         <v>4</v>
       </c>
@@ -10828,8 +10903,11 @@
       <c r="Y57" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="58" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA57" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D58" s="4">
         <v>5</v>
       </c>
@@ -10900,8 +10978,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="59" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA58" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D59" s="4">
         <v>6</v>
       </c>
@@ -10972,8 +11053,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="60" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA59" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D60" s="4">
         <v>7</v>
       </c>
@@ -11031,8 +11115,11 @@
         <v>100</v>
       </c>
       <c r="Y60" s="10"/>
-    </row>
-    <row r="61" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA60" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D61" s="4">
         <v>8</v>
       </c>
@@ -11103,8 +11190,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="62" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA61" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D62" s="4">
         <v>9</v>
       </c>
@@ -11116,7 +11206,7 @@
       <c r="X62" s="10"/>
       <c r="Y62" s="10"/>
     </row>
-    <row r="63" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D63" s="4">
         <v>10</v>
       </c>
@@ -11187,8 +11277,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="64" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA63" s="4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D64" s="4">
         <v>11</v>
       </c>
@@ -11246,8 +11339,11 @@
         <v>100</v>
       </c>
       <c r="Y64" s="10"/>
-    </row>
-    <row r="65" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA64" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D65" s="4">
         <v>12</v>
       </c>
@@ -11305,8 +11401,11 @@
         <v>100</v>
       </c>
       <c r="Y65" s="10"/>
-    </row>
-    <row r="66" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA65" s="4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D66" s="4">
         <v>13</v>
       </c>
@@ -11318,7 +11417,7 @@
       <c r="X66" s="10"/>
       <c r="Y66" s="10"/>
     </row>
-    <row r="67" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D67" s="4">
         <v>14</v>
       </c>
@@ -11389,8 +11488,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="68" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA67" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D68" s="4">
         <v>15</v>
       </c>
@@ -11402,7 +11504,7 @@
       <c r="X68" s="10"/>
       <c r="Y68" s="10"/>
     </row>
-    <row r="69" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D69" s="4">
         <v>16</v>
       </c>
@@ -11414,7 +11516,7 @@
       <c r="X69" s="10"/>
       <c r="Y69" s="10"/>
     </row>
-    <row r="70" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D70" s="4">
         <v>17</v>
       </c>
@@ -11481,8 +11583,11 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA70" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D71" s="4">
         <v>18</v>
       </c>
@@ -11553,8 +11658,11 @@
         <f t="shared" si="19"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="72" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA71" s="4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D72" s="4">
         <v>19</v>
       </c>
@@ -11621,8 +11729,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="73" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA72" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D73" s="4">
         <v>20</v>
       </c>
@@ -11634,7 +11745,7 @@
       <c r="X73" s="10"/>
       <c r="Y73" s="10"/>
     </row>
-    <row r="74" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D74" s="4">
         <v>21</v>
       </c>
@@ -11701,8 +11812,11 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA74" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D75" s="4">
         <v>22</v>
       </c>
@@ -11714,7 +11828,7 @@
       <c r="X75" s="10"/>
       <c r="Y75" s="10"/>
     </row>
-    <row r="76" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D76" s="4">
         <v>23</v>
       </c>
@@ -11785,8 +11899,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="77" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA76" s="4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D77" s="4">
         <v>24</v>
       </c>
@@ -11798,7 +11915,7 @@
       <c r="X77" s="10"/>
       <c r="Y77" s="10"/>
     </row>
-    <row r="78" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D78" s="4">
         <v>25</v>
       </c>
@@ -11810,7 +11927,7 @@
       <c r="X78" s="10"/>
       <c r="Y78" s="10"/>
     </row>
-    <row r="79" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D79" s="4">
         <v>26</v>
       </c>
@@ -11822,7 +11939,7 @@
       <c r="X79" s="10"/>
       <c r="Y79" s="10"/>
     </row>
-    <row r="80" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D80" s="4">
         <v>27</v>
       </c>
@@ -11834,7 +11951,7 @@
       <c r="X80" s="10"/>
       <c r="Y80" s="10"/>
     </row>
-    <row r="81" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D81" s="4">
         <v>28</v>
       </c>
@@ -11905,8 +12022,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="82" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA81" s="4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D82" s="4">
         <v>29</v>
       </c>
@@ -11964,8 +12084,11 @@
         <v>100</v>
       </c>
       <c r="Y82" s="10"/>
-    </row>
-    <row r="83" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA82" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D83" s="4">
         <v>30</v>
       </c>
@@ -11977,7 +12100,7 @@
       <c r="X83" s="10"/>
       <c r="Y83" s="10"/>
     </row>
-    <row r="84" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D84" s="4">
         <v>31</v>
       </c>
@@ -12035,8 +12158,11 @@
         <v>100</v>
       </c>
       <c r="Y84" s="10"/>
-    </row>
-    <row r="85" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA84" s="4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D85" s="4">
         <v>32</v>
       </c>
@@ -12103,8 +12229,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="86" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA85" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D86" s="4">
         <v>33</v>
       </c>
@@ -12116,7 +12245,7 @@
       <c r="X86" s="10"/>
       <c r="Y86" s="10"/>
     </row>
-    <row r="87" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D87" s="4">
         <v>34</v>
       </c>
@@ -12174,8 +12303,11 @@
         <v>100</v>
       </c>
       <c r="Y87" s="10"/>
-    </row>
-    <row r="88" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA87" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D88" s="4">
         <v>35</v>
       </c>
@@ -12187,7 +12319,7 @@
       <c r="X88" s="10"/>
       <c r="Y88" s="10"/>
     </row>
-    <row r="89" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D89" s="4">
         <v>36</v>
       </c>
@@ -12245,8 +12377,11 @@
         <v>100</v>
       </c>
       <c r="Y89" s="10"/>
-    </row>
-    <row r="90" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA89" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D90" s="4">
         <v>37</v>
       </c>
@@ -12258,7 +12393,7 @@
       <c r="X90" s="10"/>
       <c r="Y90" s="10"/>
     </row>
-    <row r="91" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D91" s="4">
         <v>38</v>
       </c>
@@ -12329,8 +12464,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="92" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA91" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D92" s="4">
         <v>39</v>
       </c>
@@ -12388,8 +12526,11 @@
         <v>100</v>
       </c>
       <c r="Y92" s="10"/>
-    </row>
-    <row r="93" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA92" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D93" s="4">
         <v>40</v>
       </c>
@@ -12401,7 +12542,7 @@
       <c r="X93" s="10"/>
       <c r="Y93" s="10"/>
     </row>
-    <row r="94" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D94" s="4">
         <v>41</v>
       </c>
@@ -12472,8 +12613,11 @@
         <f t="shared" si="19"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="95" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA94" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D95" s="4">
         <v>42</v>
       </c>
@@ -12485,7 +12629,7 @@
       <c r="X95" s="10"/>
       <c r="Y95" s="10"/>
     </row>
-    <row r="96" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D96" s="4">
         <v>43</v>
       </c>
@@ -12497,7 +12641,7 @@
       <c r="X96" s="10"/>
       <c r="Y96" s="10"/>
     </row>
-    <row r="97" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D97" s="4">
         <v>44</v>
       </c>
@@ -12509,7 +12653,7 @@
       <c r="X97" s="10"/>
       <c r="Y97" s="10"/>
     </row>
-    <row r="98" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D98" s="4">
         <v>46</v>
       </c>
@@ -12567,14 +12711,17 @@
         <v>100</v>
       </c>
       <c r="Y98" s="10"/>
-    </row>
-    <row r="99" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA98" s="4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="99" spans="3:27" x14ac:dyDescent="0.25">
       <c r="K99" s="10"/>
       <c r="M99" s="10"/>
       <c r="X99" s="10"/>
       <c r="Y99" s="10"/>
     </row>
-    <row r="101" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="14"/>
@@ -12598,7 +12745,7 @@
       <c r="X101" s="1"/>
       <c r="Y101" s="1"/>
     </row>
-    <row r="102" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
@@ -12622,12 +12769,12 @@
       <c r="X102" s="1"/>
       <c r="Y102" s="1"/>
     </row>
-    <row r="103" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C103" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D104" s="4">
         <v>2</v>
       </c>
@@ -12635,7 +12782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D105" s="4">
         <v>4</v>
       </c>
@@ -12693,8 +12840,11 @@
         <v>100</v>
       </c>
       <c r="Y105" s="10"/>
-    </row>
-    <row r="106" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA105" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="106" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D106" s="4">
         <v>5</v>
       </c>
@@ -12718,23 +12868,23 @@
         <v>2</v>
       </c>
       <c r="K106" s="10">
-        <f t="shared" ref="K106:K122" si="23">(J106/O106)*100</f>
+        <f t="shared" ref="K106:K121" si="23">(J106/O106)*100</f>
         <v>100</v>
       </c>
       <c r="L106" s="4">
-        <f t="shared" ref="L106:L122" si="24">G106+H106</f>
+        <f t="shared" ref="L106:L121" si="24">G106+H106</f>
         <v>1</v>
       </c>
       <c r="M106" s="10">
-        <f t="shared" ref="M106:M122" si="25">(L106/O106)*100</f>
+        <f t="shared" ref="M106:M121" si="25">(L106/O106)*100</f>
         <v>50</v>
       </c>
       <c r="N106" s="4">
-        <f t="shared" ref="N106:N122" si="26">H106+I106</f>
+        <f t="shared" ref="N106:N121" si="26">H106+I106</f>
         <v>0</v>
       </c>
       <c r="O106" s="4">
-        <f t="shared" ref="O106:O122" si="27">SUM(F106:I106)</f>
+        <f t="shared" ref="O106:O121" si="27">SUM(F106:I106)</f>
         <v>2</v>
       </c>
       <c r="R106" s="4">
@@ -12748,12 +12898,15 @@
         <v>2</v>
       </c>
       <c r="X106" s="10">
-        <f t="shared" ref="X106:X122" si="29">(W106/O106)*100</f>
+        <f t="shared" ref="X106:X121" si="29">(W106/O106)*100</f>
         <v>100</v>
       </c>
       <c r="Y106" s="10"/>
-    </row>
-    <row r="107" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA106" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D107" s="4">
         <v>6</v>
       </c>
@@ -12811,8 +12964,11 @@
         <v>100</v>
       </c>
       <c r="Y107" s="10"/>
-    </row>
-    <row r="108" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA107" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D108" s="4">
         <v>7</v>
       </c>
@@ -12870,8 +13026,11 @@
         <v>100</v>
       </c>
       <c r="Y108" s="10"/>
-    </row>
-    <row r="109" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA108" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="109" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D109" s="4">
         <v>8</v>
       </c>
@@ -12883,7 +13042,7 @@
       <c r="X109" s="10"/>
       <c r="Y109" s="10"/>
     </row>
-    <row r="110" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D110" s="4">
         <v>9</v>
       </c>
@@ -12895,7 +13054,7 @@
       <c r="X110" s="10"/>
       <c r="Y110" s="10"/>
     </row>
-    <row r="111" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D111" s="4">
         <v>10</v>
       </c>
@@ -12953,8 +13112,11 @@
         <v>100</v>
       </c>
       <c r="Y111" s="10"/>
-    </row>
-    <row r="112" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA111" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D112" s="4">
         <v>11</v>
       </c>
@@ -12966,7 +13128,7 @@
       <c r="X112" s="10"/>
       <c r="Y112" s="10"/>
     </row>
-    <row r="113" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D113" s="4">
         <v>12</v>
       </c>
@@ -12978,7 +13140,7 @@
       <c r="X113" s="10"/>
       <c r="Y113" s="10"/>
     </row>
-    <row r="114" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D114" s="4">
         <v>13</v>
       </c>
@@ -13046,11 +13208,14 @@
         <v>100</v>
       </c>
       <c r="Y114" s="10">
-        <f t="shared" ref="Y114:Y122" si="31">(V114/N114)*100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="115" spans="3:25" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Y114:Y121" si="31">(V114/N114)*100</f>
+        <v>100</v>
+      </c>
+      <c r="AA114" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="115" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D115" s="4">
         <v>14</v>
       </c>
@@ -13108,8 +13273,11 @@
         <v>100</v>
       </c>
       <c r="Y115" s="10"/>
-    </row>
-    <row r="116" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA115" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D116" s="4">
         <v>15</v>
       </c>
@@ -13121,7 +13289,7 @@
       <c r="X116" s="10"/>
       <c r="Y116" s="10"/>
     </row>
-    <row r="117" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D117" s="4">
         <v>16</v>
       </c>
@@ -13133,7 +13301,7 @@
       <c r="X117" s="10"/>
       <c r="Y117" s="10"/>
     </row>
-    <row r="118" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D118" s="4">
         <v>17</v>
       </c>
@@ -13145,7 +13313,7 @@
       <c r="X118" s="10"/>
       <c r="Y118" s="10"/>
     </row>
-    <row r="119" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D119" s="4">
         <v>19</v>
       </c>
@@ -13212,8 +13380,11 @@
         <f t="shared" si="31"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="120" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA119" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D120" s="4">
         <v>20</v>
       </c>
@@ -13274,8 +13445,11 @@
         <v>100</v>
       </c>
       <c r="Y120" s="10"/>
-    </row>
-    <row r="121" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA120" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D121" s="4">
         <v>21</v>
       </c>
@@ -13346,15 +13520,18 @@
         <f t="shared" si="31"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="122" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA121" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="122" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D122" s="12"/>
       <c r="K122" s="10"/>
       <c r="M122" s="10"/>
       <c r="X122" s="10"/>
       <c r="Y122" s="10"/>
     </row>
-    <row r="124" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="14"/>
@@ -13378,7 +13555,7 @@
       <c r="X124" s="1"/>
       <c r="Y124" s="1"/>
     </row>
-    <row r="125" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -13402,7 +13579,7 @@
       <c r="X125" s="1"/>
       <c r="Y125" s="1"/>
     </row>
-    <row r="126" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C126" s="4" t="s">
         <v>42</v>
       </c>
@@ -13413,7 +13590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D127" s="4">
         <v>2</v>
       </c>
@@ -13421,7 +13598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D128" s="4">
         <v>3</v>
       </c>
@@ -13479,8 +13656,11 @@
         <v>100</v>
       </c>
       <c r="Y128" s="10"/>
-    </row>
-    <row r="129" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA128" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D129" s="4">
         <v>4</v>
       </c>
@@ -13504,7 +13684,7 @@
         <v>5</v>
       </c>
       <c r="K129" s="10">
-        <f t="shared" ref="K129:K147" si="35">(J129/O129)*100</f>
+        <f t="shared" ref="K129:K146" si="35">(J129/O129)*100</f>
         <v>100</v>
       </c>
       <c r="L129" s="6">
@@ -13512,15 +13692,15 @@
         <v>1</v>
       </c>
       <c r="M129" s="10">
-        <f t="shared" ref="M129:M147" si="37">(L129/O129)*100</f>
+        <f t="shared" ref="M129:M146" si="37">(L129/O129)*100</f>
         <v>20</v>
       </c>
       <c r="N129" s="4">
-        <f t="shared" ref="N129:N147" si="38">H129+I129</f>
+        <f t="shared" ref="N129:N146" si="38">H129+I129</f>
         <v>0</v>
       </c>
       <c r="O129" s="4">
-        <f t="shared" ref="O129:O147" si="39">SUM(F129:I129)</f>
+        <f t="shared" ref="O129:O146" si="39">SUM(F129:I129)</f>
         <v>5</v>
       </c>
       <c r="R129" s="4">
@@ -13530,16 +13710,19 @@
         <v>1</v>
       </c>
       <c r="W129" s="4">
-        <f t="shared" ref="W129:W147" si="40">SUM(R129:U129)</f>
+        <f t="shared" ref="W129:W146" si="40">SUM(R129:U129)</f>
         <v>5</v>
       </c>
       <c r="X129" s="10">
-        <f t="shared" ref="X129:X147" si="41">(W129/O129)*100</f>
+        <f t="shared" ref="X129:X146" si="41">(W129/O129)*100</f>
         <v>100</v>
       </c>
       <c r="Y129" s="10"/>
-    </row>
-    <row r="130" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA129" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D130" s="4">
         <v>5</v>
       </c>
@@ -13597,8 +13780,11 @@
         <v>100</v>
       </c>
       <c r="Y130" s="10"/>
-    </row>
-    <row r="131" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA130" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D131" s="4">
         <v>6</v>
       </c>
@@ -13656,8 +13842,11 @@
         <v>100</v>
       </c>
       <c r="Y131" s="10"/>
-    </row>
-    <row r="132" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA131" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D132" s="4">
         <v>7</v>
       </c>
@@ -13669,7 +13858,7 @@
       <c r="X132" s="10"/>
       <c r="Y132" s="10"/>
     </row>
-    <row r="133" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D133" s="4">
         <v>8</v>
       </c>
@@ -13727,8 +13916,11 @@
         <v>100</v>
       </c>
       <c r="Y133" s="10"/>
-    </row>
-    <row r="134" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA133" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="134" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D134" s="4">
         <v>9</v>
       </c>
@@ -13740,7 +13932,7 @@
       <c r="X134" s="10"/>
       <c r="Y134" s="10"/>
     </row>
-    <row r="135" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D135" s="4">
         <v>10</v>
       </c>
@@ -13752,7 +13944,7 @@
       <c r="X135" s="10"/>
       <c r="Y135" s="10"/>
     </row>
-    <row r="136" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D136" s="4">
         <v>11</v>
       </c>
@@ -13819,8 +14011,11 @@
         <f>(V136/N136)*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="137" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA136" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="137" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D137" s="4">
         <v>13</v>
       </c>
@@ -13878,8 +14073,11 @@
         <v>100</v>
       </c>
       <c r="Y137" s="10"/>
-    </row>
-    <row r="138" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA137" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D138" s="4">
         <v>14</v>
       </c>
@@ -13891,7 +14089,7 @@
       <c r="X138" s="10"/>
       <c r="Y138" s="10"/>
     </row>
-    <row r="139" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D139" s="4">
         <v>15</v>
       </c>
@@ -13959,11 +14157,14 @@
         <v>100</v>
       </c>
       <c r="Y139" s="10">
-        <f t="shared" ref="Y139:Y147" si="43">(V139/N139)*100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="140" spans="4:25" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Y139:Y142" si="43">(V139/N139)*100</f>
+        <v>100</v>
+      </c>
+      <c r="AA139" s="4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="140" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D140" s="4">
         <v>16</v>
       </c>
@@ -14021,8 +14222,11 @@
         <v>100</v>
       </c>
       <c r="Y140" s="10"/>
-    </row>
-    <row r="141" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA140" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D141" s="4">
         <v>17</v>
       </c>
@@ -14080,8 +14284,11 @@
         <v>100</v>
       </c>
       <c r="Y141" s="10"/>
-    </row>
-    <row r="142" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA141" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D142" s="4">
         <v>18</v>
       </c>
@@ -14152,8 +14359,11 @@
         <f t="shared" si="43"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="143" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA142" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D143" s="4">
         <v>19</v>
       </c>
@@ -14165,7 +14375,7 @@
       <c r="X143" s="10"/>
       <c r="Y143" s="10"/>
     </row>
-    <row r="144" spans="4:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D144" s="4">
         <v>21</v>
       </c>
@@ -14223,8 +14433,11 @@
         <v>100</v>
       </c>
       <c r="Y144" s="10"/>
-    </row>
-    <row r="145" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA144" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="145" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D145" s="4">
         <v>22</v>
       </c>
@@ -14282,8 +14495,11 @@
         <v>100</v>
       </c>
       <c r="Y145" s="10"/>
-    </row>
-    <row r="146" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA145" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D146" s="4">
         <v>23</v>
       </c>
@@ -14341,8 +14557,11 @@
         <v>100</v>
       </c>
       <c r="Y146" s="10"/>
-    </row>
-    <row r="147" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="AA146" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="4:27" x14ac:dyDescent="0.25">
       <c r="J147" s="6"/>
       <c r="K147" s="10"/>
       <c r="L147" s="6"/>
@@ -17718,7 +17937,7 @@
         <v>8</v>
       </c>
       <c r="H132" s="10">
-        <f t="shared" ref="H132:H155" si="35">F132/I132*100</f>
+        <f t="shared" ref="H132:H151" si="35">F132/I132*100</f>
         <v>76.470588235294116</v>
       </c>
       <c r="I132" s="4">
@@ -17736,11 +17955,11 @@
         <v>27</v>
       </c>
       <c r="P132" s="10">
-        <f t="shared" ref="P132:P155" si="38">(O132/I132)*100</f>
+        <f t="shared" ref="P132:P151" si="38">(O132/I132)*100</f>
         <v>79.411764705882348</v>
       </c>
       <c r="Q132" s="10">
-        <f t="shared" ref="Q132:Q155" si="39">(N132/G132)*100</f>
+        <f t="shared" ref="Q132:Q151" si="39">(N132/G132)*100</f>
         <v>12.5</v>
       </c>
     </row>

</xml_diff>